<commit_message>
alert and deny vacation request with accepted date for another user
</commit_message>
<xml_diff>
--- a/media/table_data.xlsx
+++ b/media/table_data.xlsx
@@ -413,28 +413,58 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Username</t>
+          <t>UŻYTKOWNIK</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Start Date</t>
+          <t>DATA WNIOSKU</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>End Date</t>
+          <t>TYP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>OD</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>DO</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>ILOŚĆ DNI</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AKCEPTACJA</t>
         </is>
       </c>
     </row>
@@ -449,9 +479,27 @@
           <t>2023-06-20</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>wypoczynkowy</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2023-06-20</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>17</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Tak</t>
         </is>
       </c>
     </row>
@@ -466,9 +514,27 @@
           <t>2023-06-20</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>wypoczynkowy</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2023-06-20</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>2023-06-21</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Tak</t>
         </is>
       </c>
     </row>
@@ -483,9 +549,27 @@
           <t>2023-06-20</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>wypoczynkowy</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2023-06-20</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>2023-06-22</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nie</t>
         </is>
       </c>
     </row>
@@ -500,9 +584,27 @@
           <t>2023-06-21</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>wypoczynkowy</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2023-06-21</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>2023-06-22</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nie</t>
         </is>
       </c>
     </row>

</xml_diff>